<commit_message>
Corrigindo uma Análise dos Clusters - Data Masters
</commit_message>
<xml_diff>
--- a/Apresentação.xlsx
+++ b/Apresentação.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leova\Desktop\Projetos\00_DataMaster\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F665B46-5ACB-4A13-9B49-8E478A438DA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4587DADD-E919-44B0-9C88-198841894CDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="16200" windowHeight="19200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -586,7 +586,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -606,10 +606,7 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -618,42 +615,15 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -666,7 +636,7 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -700,15 +670,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -717,9 +678,6 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="13" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -728,6 +686,45 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="9" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1013,7 +1010,7 @@
   <dimension ref="F5:AG57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J40" workbookViewId="0">
-      <selection activeCell="X49" sqref="X49"/>
+      <selection activeCell="Q54" sqref="Q54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1082,31 +1079,31 @@
       <c r="U5" s="1">
         <v>201612</v>
       </c>
-      <c r="Y5" s="23" t="s">
+      <c r="Y5" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="Z5" s="24" t="s">
+      <c r="Z5" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="AA5" s="24" t="s">
+      <c r="AA5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="AB5" s="24" t="s">
+      <c r="AB5" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="AC5" s="24" t="s">
+      <c r="AC5" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="AD5" s="24" t="s">
+      <c r="AD5" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="AE5" s="24" t="s">
+      <c r="AE5" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="AF5" s="24" t="s">
+      <c r="AF5" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="AG5" s="25" t="s">
+      <c r="AG5" s="15" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1114,35 +1111,35 @@
       <c r="F6" s="1">
         <v>201601</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="37" t="s">
         <v>2</v>
       </c>
       <c r="X6" s="2"/>
-      <c r="Y6" s="9" t="s">
+      <c r="Y6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="Z6" s="10" t="s">
+      <c r="Z6" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="AA6" s="10" t="s">
+      <c r="AA6" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="AB6" s="10" t="s">
+      <c r="AB6" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="AC6" s="10" t="s">
+      <c r="AC6" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="AD6" s="10" t="s">
+      <c r="AD6" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="AE6" s="10" t="s">
+      <c r="AE6" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="AF6" s="10" t="s">
+      <c r="AF6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="AG6" s="11" t="s">
+      <c r="AG6" s="38" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1150,33 +1147,33 @@
       <c r="F7" s="1">
         <v>201602</v>
       </c>
-      <c r="G7" s="7"/>
+      <c r="G7" s="37"/>
       <c r="X7" s="2"/>
-      <c r="Y7" s="12" t="s">
+      <c r="Y7" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="Z7" s="8" t="s">
+      <c r="Z7" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="AA7" s="8" t="s">
+      <c r="AA7" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="AB7" s="8" t="s">
+      <c r="AB7" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="AC7" s="8" t="s">
+      <c r="AC7" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="AD7" s="8" t="s">
+      <c r="AD7" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="AE7" s="8" t="s">
+      <c r="AE7" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="AF7" s="8" t="s">
+      <c r="AF7" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="AG7" s="13"/>
+      <c r="AG7" s="39"/>
     </row>
     <row r="8" spans="6:33" ht="16.5" x14ac:dyDescent="0.25">
       <c r="F8" s="1">
@@ -1186,31 +1183,31 @@
         <v>3</v>
       </c>
       <c r="X8" s="2"/>
-      <c r="Y8" s="14" t="s">
+      <c r="Y8" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="Z8" s="15" t="s">
+      <c r="Z8" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="AA8" s="15" t="s">
+      <c r="AA8" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="AB8" s="15" t="s">
+      <c r="AB8" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="AC8" s="15" t="s">
+      <c r="AC8" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="AD8" s="15" t="s">
+      <c r="AD8" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="AE8" s="15" t="s">
+      <c r="AE8" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="AF8" s="15" t="s">
+      <c r="AF8" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="AG8" s="16"/>
+      <c r="AG8" s="40"/>
     </row>
     <row r="9" spans="6:33" ht="16.5" x14ac:dyDescent="0.25">
       <c r="F9" s="1">
@@ -1220,31 +1217,31 @@
         <v>3</v>
       </c>
       <c r="X9" s="2"/>
-      <c r="Y9" s="9" t="s">
+      <c r="Y9" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="Z9" s="10" t="s">
+      <c r="Z9" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="AA9" s="10" t="s">
+      <c r="AA9" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="AB9" s="10" t="s">
+      <c r="AB9" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="AC9" s="10" t="s">
+      <c r="AC9" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="AD9" s="10" t="s">
+      <c r="AD9" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="AE9" s="10" t="s">
+      <c r="AE9" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="AF9" s="10" t="s">
+      <c r="AF9" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="AG9" s="17" t="s">
+      <c r="AG9" s="41" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1256,31 +1253,31 @@
         <v>3</v>
       </c>
       <c r="X10" s="2"/>
-      <c r="Y10" s="12" t="s">
+      <c r="Y10" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="Z10" s="8" t="s">
+      <c r="Z10" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="AA10" s="8" t="s">
+      <c r="AA10" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="AB10" s="8" t="s">
+      <c r="AB10" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="AC10" s="8" t="s">
+      <c r="AC10" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="AD10" s="8" t="s">
+      <c r="AD10" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="AE10" s="8" t="s">
+      <c r="AE10" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="AF10" s="8" t="s">
+      <c r="AF10" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="AG10" s="18"/>
+      <c r="AG10" s="42"/>
     </row>
     <row r="11" spans="6:33" ht="16.5" x14ac:dyDescent="0.25">
       <c r="F11" s="1">
@@ -1290,31 +1287,31 @@
         <v>3</v>
       </c>
       <c r="X11" s="2"/>
-      <c r="Y11" s="14" t="s">
+      <c r="Y11" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="Z11" s="15" t="s">
+      <c r="Z11" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="AA11" s="15" t="s">
+      <c r="AA11" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="AB11" s="15" t="s">
+      <c r="AB11" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="AC11" s="15" t="s">
+      <c r="AC11" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="AD11" s="15" t="s">
+      <c r="AD11" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="AE11" s="15" t="s">
+      <c r="AE11" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="AF11" s="15" t="s">
+      <c r="AF11" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="AG11" s="19"/>
+      <c r="AG11" s="43"/>
     </row>
     <row r="12" spans="6:33" ht="16.5" x14ac:dyDescent="0.25">
       <c r="F12" s="1">
@@ -1324,31 +1321,31 @@
         <v>3</v>
       </c>
       <c r="X12" s="2"/>
-      <c r="Y12" s="9" t="s">
+      <c r="Y12" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="Z12" s="10" t="s">
+      <c r="Z12" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="AA12" s="10" t="s">
+      <c r="AA12" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="AB12" s="10" t="s">
+      <c r="AB12" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="AC12" s="10" t="s">
+      <c r="AC12" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="AD12" s="10" t="s">
+      <c r="AD12" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="AE12" s="10" t="s">
+      <c r="AE12" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="AF12" s="10" t="s">
+      <c r="AF12" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="AG12" s="20" t="s">
+      <c r="AG12" s="44" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1360,31 +1357,31 @@
         <v>3</v>
       </c>
       <c r="X13" s="2"/>
-      <c r="Y13" s="12" t="s">
+      <c r="Y13" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="Z13" s="8" t="s">
+      <c r="Z13" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="AA13" s="8" t="s">
+      <c r="AA13" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="AB13" s="8" t="s">
+      <c r="AB13" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="AC13" s="8" t="s">
+      <c r="AC13" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="AD13" s="8" t="s">
+      <c r="AD13" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="AE13" s="8" t="s">
+      <c r="AE13" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="AF13" s="8" t="s">
+      <c r="AF13" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="AG13" s="21"/>
+      <c r="AG13" s="45"/>
     </row>
     <row r="14" spans="6:33" ht="16.5" x14ac:dyDescent="0.25">
       <c r="F14" s="1">
@@ -1394,37 +1391,37 @@
         <v>4</v>
       </c>
       <c r="X14" s="2"/>
-      <c r="Y14" s="14" t="s">
+      <c r="Y14" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="Z14" s="15" t="s">
+      <c r="Z14" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="AA14" s="15" t="s">
+      <c r="AA14" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="AB14" s="15" t="s">
+      <c r="AB14" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="AC14" s="15" t="s">
+      <c r="AC14" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="AD14" s="15" t="s">
+      <c r="AD14" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="AE14" s="15" t="s">
+      <c r="AE14" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="AF14" s="15" t="s">
+      <c r="AF14" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="AG14" s="22"/>
+      <c r="AG14" s="46"/>
     </row>
     <row r="15" spans="6:33" x14ac:dyDescent="0.25">
       <c r="F15" s="1">
         <v>201610</v>
       </c>
-      <c r="G15" s="7" t="s">
+      <c r="G15" s="37" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1432,172 +1429,172 @@
       <c r="F16" s="1">
         <v>201611</v>
       </c>
-      <c r="G16" s="7"/>
+      <c r="G16" s="37"/>
     </row>
     <row r="17" spans="6:33" x14ac:dyDescent="0.25">
       <c r="F17" s="1">
         <v>201612</v>
       </c>
-      <c r="G17" s="7"/>
+      <c r="G17" s="37"/>
     </row>
     <row r="18" spans="6:33" x14ac:dyDescent="0.25">
-      <c r="Y18" s="26" t="s">
+      <c r="Y18" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="Z18" s="26" t="s">
+      <c r="Z18" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="AA18" s="26" t="s">
+      <c r="AA18" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="AB18" s="26" t="s">
+      <c r="AB18" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="AC18" s="26" t="s">
+      <c r="AC18" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="AD18" s="26" t="s">
+      <c r="AD18" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="AE18" s="26" t="s">
+      <c r="AE18" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="AF18" s="26" t="s">
+      <c r="AF18" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="AG18" s="26" t="s">
+      <c r="AG18" s="16" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="19" spans="6:33" ht="21" x14ac:dyDescent="0.25">
-      <c r="K19" s="34">
+      <c r="K19" s="24">
         <v>0</v>
       </c>
-      <c r="L19" s="35">
+      <c r="L19" s="25">
         <v>14.4</v>
       </c>
-      <c r="M19" s="35">
+      <c r="M19" s="25">
         <v>24.5</v>
       </c>
-      <c r="N19" s="35">
+      <c r="N19" s="25">
         <v>555</v>
       </c>
-      <c r="O19" s="35">
+      <c r="O19" s="25">
         <v>121.5</v>
       </c>
-      <c r="Y19" s="12" t="s">
+      <c r="Y19" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="Z19" s="8" t="s">
+      <c r="Z19" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="AA19" s="8" t="s">
+      <c r="AA19" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="AB19" s="8" t="s">
+      <c r="AB19" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="AC19" s="8" t="s">
+      <c r="AC19" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="AD19" s="8" t="s">
+      <c r="AD19" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="AE19" s="8" t="s">
+      <c r="AE19" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="AF19" s="27" t="s">
+      <c r="AF19" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="AG19" s="28" t="s">
+      <c r="AG19" s="18" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="20" spans="6:33" ht="21" x14ac:dyDescent="0.25">
-      <c r="K20" s="34">
+      <c r="K20" s="24">
         <v>1</v>
       </c>
-      <c r="L20" s="35">
+      <c r="L20" s="25">
         <v>22.9</v>
       </c>
-      <c r="M20" s="35">
+      <c r="M20" s="25">
         <v>40.799999999999997</v>
       </c>
-      <c r="N20" s="35">
+      <c r="N20" s="25">
         <v>1552.4</v>
       </c>
-      <c r="O20" s="35">
+      <c r="O20" s="25">
         <v>138.9</v>
       </c>
-      <c r="Y20" s="12" t="s">
+      <c r="Y20" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="Z20" s="8" t="s">
+      <c r="Z20" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="AA20" s="8" t="s">
+      <c r="AA20" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="AB20" s="8" t="s">
+      <c r="AB20" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="AC20" s="8" t="s">
+      <c r="AC20" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="AD20" s="8" t="s">
+      <c r="AD20" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="AE20" s="8" t="s">
+      <c r="AE20" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="AF20" s="27" t="s">
+      <c r="AF20" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="AG20" s="28" t="s">
+      <c r="AG20" s="18" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="21" spans="6:33" ht="21" x14ac:dyDescent="0.25">
-      <c r="K21" s="34">
+      <c r="K21" s="24">
         <v>2</v>
       </c>
-      <c r="L21" s="35">
+      <c r="L21" s="25">
         <v>28.3</v>
       </c>
-      <c r="M21" s="35">
+      <c r="M21" s="25">
         <v>51.4</v>
       </c>
-      <c r="N21" s="35">
+      <c r="N21" s="25">
         <v>683</v>
       </c>
-      <c r="O21" s="35">
+      <c r="O21" s="25">
         <v>140.6</v>
       </c>
-      <c r="Y21" s="14" t="s">
+      <c r="Y21" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="Z21" s="15" t="s">
+      <c r="Z21" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="AA21" s="15" t="s">
+      <c r="AA21" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="AB21" s="15" t="s">
+      <c r="AB21" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="AC21" s="15" t="s">
+      <c r="AC21" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="AD21" s="15" t="s">
+      <c r="AD21" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="AE21" s="15" t="s">
+      <c r="AE21" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="AF21" s="29" t="s">
+      <c r="AF21" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="AG21" s="30" t="s">
+      <c r="AG21" s="20" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1660,34 +1657,34 @@
       </c>
     </row>
     <row r="28" spans="6:33" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="K28" s="33">
+      <c r="K28" s="23">
         <v>0</v>
       </c>
-      <c r="L28" s="36">
+      <c r="L28" s="26">
         <v>14.4</v>
       </c>
-      <c r="M28" s="40"/>
-      <c r="N28" s="44"/>
-      <c r="O28" s="44"/>
+      <c r="M28" s="36"/>
+      <c r="N28" s="34"/>
+      <c r="O28" s="34"/>
     </row>
     <row r="29" spans="6:33" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="K29" s="33">
+      <c r="K29" s="23">
         <v>1</v>
       </c>
-      <c r="L29" s="42"/>
-      <c r="M29" s="37">
+      <c r="L29" s="29"/>
+      <c r="M29" s="27">
         <v>22.9</v>
       </c>
-      <c r="N29" s="40"/>
-      <c r="O29" s="39"/>
+      <c r="N29" s="36"/>
+      <c r="O29" s="34"/>
     </row>
     <row r="30" spans="6:33" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="K30" s="33">
+      <c r="K30" s="23">
         <v>2</v>
       </c>
-      <c r="L30" s="39"/>
-      <c r="M30" s="41"/>
-      <c r="N30" s="38">
+      <c r="L30" s="34"/>
+      <c r="M30" s="35"/>
+      <c r="N30" s="28">
         <v>28.3</v>
       </c>
       <c r="Y30" s="4" t="s">
@@ -1698,10 +1695,10 @@
       </c>
     </row>
     <row r="31" spans="6:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L31" s="39"/>
-      <c r="M31" s="39"/>
-      <c r="N31" s="39"/>
-      <c r="O31" s="39"/>
+      <c r="L31" s="34"/>
+      <c r="M31" s="34"/>
+      <c r="N31" s="34"/>
+      <c r="O31" s="34"/>
       <c r="Y31" s="4" t="s">
         <v>55</v>
       </c>
@@ -1710,7 +1707,7 @@
       </c>
     </row>
     <row r="32" spans="6:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L32" s="43"/>
+      <c r="L32" s="30"/>
       <c r="Y32" s="4" t="s">
         <v>56</v>
       </c>
@@ -1727,15 +1724,15 @@
       </c>
     </row>
     <row r="34" spans="11:33" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="K34" s="33">
+      <c r="K34" s="23">
         <v>0</v>
       </c>
-      <c r="L34" s="36">
+      <c r="L34" s="26">
         <v>24.5</v>
       </c>
-      <c r="M34" s="40"/>
-      <c r="N34" s="44"/>
-      <c r="O34" s="44"/>
+      <c r="M34" s="36"/>
+      <c r="N34" s="34"/>
+      <c r="O34" s="34"/>
       <c r="Y34" s="4" t="s">
         <v>58</v>
       </c>
@@ -1744,15 +1741,15 @@
       </c>
     </row>
     <row r="35" spans="11:33" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="K35" s="33">
+      <c r="K35" s="23">
         <v>1</v>
       </c>
-      <c r="L35" s="42"/>
-      <c r="M35" s="37">
+      <c r="L35" s="29"/>
+      <c r="M35" s="27">
         <v>40.799999999999997</v>
       </c>
-      <c r="N35" s="40"/>
-      <c r="O35" s="39"/>
+      <c r="N35" s="36"/>
+      <c r="O35" s="34"/>
       <c r="Y35" s="4" t="s">
         <v>59</v>
       </c>
@@ -1761,12 +1758,12 @@
       </c>
     </row>
     <row r="36" spans="11:33" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="K36" s="33">
+      <c r="K36" s="23">
         <v>2</v>
       </c>
-      <c r="L36" s="39"/>
-      <c r="M36" s="41"/>
-      <c r="N36" s="38">
+      <c r="L36" s="34"/>
+      <c r="M36" s="35"/>
+      <c r="N36" s="28">
         <v>51.4</v>
       </c>
       <c r="Y36" s="4" t="s">
@@ -1793,243 +1790,252 @@
       </c>
     </row>
     <row r="40" spans="11:33" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="K40" s="33">
+      <c r="K40" s="23">
         <v>0</v>
       </c>
-      <c r="L40" s="36">
+      <c r="L40" s="26">
         <v>555</v>
       </c>
-      <c r="M40" s="40"/>
-      <c r="N40" s="44"/>
-      <c r="O40" s="44"/>
+      <c r="M40" s="36"/>
+      <c r="N40" s="34"/>
+      <c r="O40" s="34"/>
     </row>
     <row r="41" spans="11:33" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="K41" s="33">
+      <c r="K41" s="23">
         <v>1</v>
       </c>
-      <c r="L41" s="42"/>
-      <c r="M41" s="38">
+      <c r="L41" s="29"/>
+      <c r="M41" s="28">
         <v>1552</v>
       </c>
-      <c r="N41" s="40"/>
-      <c r="O41" s="39"/>
+      <c r="N41" s="36"/>
+      <c r="O41" s="34"/>
     </row>
     <row r="42" spans="11:33" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="K42" s="33">
+      <c r="K42" s="23">
         <v>2</v>
       </c>
-      <c r="L42" s="39"/>
-      <c r="M42" s="41"/>
-      <c r="N42" s="37">
+      <c r="L42" s="34"/>
+      <c r="M42" s="35"/>
+      <c r="N42" s="27">
         <v>683</v>
       </c>
-      <c r="Y42" s="26" t="s">
+      <c r="Y42" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="Z42" s="26" t="s">
+      <c r="Z42" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="AA42" s="26" t="s">
+      <c r="AA42" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="AB42" s="26" t="s">
+      <c r="AB42" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="AC42" s="26" t="s">
+      <c r="AC42" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="AD42" s="26" t="s">
+      <c r="AD42" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="AE42" s="26" t="s">
+      <c r="AE42" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="AF42" s="26" t="s">
+      <c r="AF42" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="AG42" s="26" t="s">
+      <c r="AG42" s="16" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="43" spans="11:33" x14ac:dyDescent="0.25">
-      <c r="Y43" s="12" t="s">
+      <c r="Y43" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="Z43" s="8" t="s">
+      <c r="Z43" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="AA43" s="8" t="s">
+      <c r="AA43" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="AB43" s="8" t="s">
+      <c r="AB43" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="AC43" s="8" t="s">
+      <c r="AC43" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="AD43" s="8" t="s">
+      <c r="AD43" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="AE43" s="8" t="s">
+      <c r="AE43" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="AF43" s="27" t="s">
+      <c r="AF43" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="AG43" s="31" t="s">
+      <c r="AG43" s="21" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="44" spans="11:33" x14ac:dyDescent="0.25">
-      <c r="Y44" s="14" t="s">
+      <c r="Y44" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="Z44" s="15" t="s">
+      <c r="Z44" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="AA44" s="15" t="s">
+      <c r="AA44" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="AB44" s="15" t="s">
+      <c r="AB44" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="AC44" s="15" t="s">
+      <c r="AC44" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="AD44" s="15" t="s">
+      <c r="AD44" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="AE44" s="15" t="s">
+      <c r="AE44" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="AF44" s="29" t="s">
+      <c r="AF44" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="AG44" s="32" t="s">
+      <c r="AG44" s="22" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="46" spans="11:33" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="K46" s="33">
+      <c r="K46" s="23">
         <v>0</v>
       </c>
-      <c r="L46" s="36">
+      <c r="L46" s="26">
         <v>121.5</v>
       </c>
-      <c r="M46" s="40"/>
-      <c r="N46" s="44"/>
-      <c r="O46" s="44"/>
+      <c r="M46" s="36"/>
+      <c r="N46" s="34"/>
+      <c r="O46" s="34"/>
     </row>
     <row r="47" spans="11:33" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="K47" s="33">
+      <c r="K47" s="23">
         <v>1</v>
       </c>
-      <c r="L47" s="42"/>
-      <c r="M47" s="37">
+      <c r="L47" s="29"/>
+      <c r="M47" s="27">
         <v>138</v>
       </c>
-      <c r="N47" s="40"/>
-      <c r="O47" s="39"/>
+      <c r="N47" s="36"/>
+      <c r="O47" s="34"/>
     </row>
     <row r="48" spans="11:33" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="K48" s="33">
+      <c r="K48" s="23">
         <v>2</v>
       </c>
-      <c r="L48" s="39"/>
-      <c r="M48" s="41"/>
-      <c r="N48" s="38">
+      <c r="L48" s="34"/>
+      <c r="M48" s="35"/>
+      <c r="N48" s="28">
         <v>140.6</v>
       </c>
     </row>
     <row r="54" spans="11:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="K54" s="33">
+      <c r="K54" s="23">
         <v>0</v>
       </c>
-      <c r="L54" s="45">
+      <c r="L54" s="31">
         <v>0.56000000000000005</v>
       </c>
-      <c r="M54" s="45">
+      <c r="M54" s="31">
         <v>0.26</v>
       </c>
-      <c r="N54" s="45">
+      <c r="N54" s="31">
         <v>0.17</v>
       </c>
-      <c r="O54" s="33">
+      <c r="O54" s="23">
         <v>0</v>
       </c>
-      <c r="P54" s="46">
+      <c r="P54" s="32">
         <v>-21</v>
       </c>
-      <c r="Q54" s="47">
+      <c r="Q54" s="33">
         <v>1207</v>
       </c>
     </row>
     <row r="55" spans="11:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="K55" s="33">
+      <c r="K55" s="23">
         <v>1</v>
       </c>
-      <c r="L55" s="45">
+      <c r="L55" s="31">
         <v>0.25</v>
       </c>
-      <c r="M55" s="45">
+      <c r="M55" s="31">
         <v>0.31</v>
       </c>
-      <c r="N55" s="45">
+      <c r="N55" s="31">
         <v>0.44</v>
       </c>
-      <c r="O55" s="33">
+      <c r="O55" s="23">
         <v>1</v>
       </c>
-      <c r="P55" s="46">
+      <c r="P55" s="32">
         <v>-3</v>
       </c>
-      <c r="Q55" s="47">
+      <c r="Q55" s="33">
         <v>1274</v>
       </c>
     </row>
     <row r="56" spans="11:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="K56" s="33">
+      <c r="K56" s="23">
         <v>2</v>
       </c>
-      <c r="L56" s="45">
+      <c r="L56" s="31">
         <v>0.12</v>
       </c>
-      <c r="M56" s="45">
+      <c r="M56" s="31">
         <v>0.41</v>
       </c>
-      <c r="N56" s="45">
+      <c r="N56" s="31">
         <v>0.47</v>
       </c>
-      <c r="O56" s="33">
+      <c r="O56" s="23">
         <v>2</v>
       </c>
-      <c r="P56" s="46">
+      <c r="P56" s="32">
         <v>-32</v>
       </c>
-      <c r="Q56" s="47">
+      <c r="Q56" s="33">
         <v>1214</v>
       </c>
     </row>
     <row r="57" spans="11:17" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="L57" s="33" t="s">
+      <c r="L57" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="M57" s="33" t="s">
+      <c r="M57" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="N57" s="33" t="s">
+      <c r="N57" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="O57" s="33"/>
-      <c r="P57" s="33" t="s">
+      <c r="O57" s="23"/>
+      <c r="P57" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="Q57" s="33" t="s">
+      <c r="Q57" s="23" t="s">
         <v>77</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="AG6:AG8"/>
+    <mergeCell ref="AG9:AG11"/>
+    <mergeCell ref="AG12:AG14"/>
+    <mergeCell ref="N29:O29"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="L31:O31"/>
+    <mergeCell ref="M28:O28"/>
+    <mergeCell ref="G15:G17"/>
     <mergeCell ref="L42:M42"/>
     <mergeCell ref="M46:O46"/>
     <mergeCell ref="N47:O47"/>
@@ -2039,18 +2045,21 @@
     <mergeCell ref="L36:M36"/>
     <mergeCell ref="M40:O40"/>
     <mergeCell ref="N41:O41"/>
-    <mergeCell ref="N29:O29"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="L31:O31"/>
-    <mergeCell ref="M28:O28"/>
-    <mergeCell ref="G15:G17"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="AG6:AG8"/>
-    <mergeCell ref="AG9:AG11"/>
-    <mergeCell ref="AG12:AG14"/>
   </mergeCells>
   <conditionalFormatting sqref="L19:L21">
     <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L54:N56">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2097,18 +2106,6 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L54:N56">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="W60">
     <cfRule type="iconSet" priority="1">
       <iconSet>

</xml_diff>